<commit_message>
New index were included and data structure was improved
</commit_message>
<xml_diff>
--- a/APM/DATA/IEEE39_Asset_Data.xlsx
+++ b/APM/DATA/IEEE39_Asset_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LOAD_TAGS" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="224">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -466,6 +466,111 @@
   </si>
   <si>
     <t xml:space="preserve">Bus_39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_04_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN _06_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN _10_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_10_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_13_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_16_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_16_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_16_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_26_28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_26_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_28_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_23_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_22_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_03_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_08_09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_07_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_02_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_01_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_25_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_17_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_26_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_17_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_16_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_15_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_14_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_04_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_03_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_02_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_01_39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_09_39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_05_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_05_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_06_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN_21_22</t>
   </si>
   <si>
     <t xml:space="preserve">Lon</t>
@@ -766,7 +871,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -855,6 +960,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -879,7 +988,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Excel Built-in Comma [0]" xfId="20"/>
+    <cellStyle name="Excel Built-in Comma [0] 1" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -952,7 +1061,7 @@
   <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="1" sqref="B2:B105 E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2091,22 +2200,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="16.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.17"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
@@ -3524,6 +3633,686 @@
       </c>
       <c r="F71" s="20" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="20" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D72" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F72" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="20" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D73" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F73" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="20" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D74" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F74" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="20" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D75" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F75" s="22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="20" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D76" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E76" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F76" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="20" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D77" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E77" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F77" s="22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="20" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D78" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E78" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F78" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="20" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D79" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F79" s="22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="20" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D80" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E80" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F80" s="22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="20" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D81" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E81" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F81" s="22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="20" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D82" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E82" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F82" s="22" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="20" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D83" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E83" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F83" s="22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="20" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D84" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E84" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F84" s="22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="20" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D85" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E85" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F85" s="22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="20" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D86" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E86" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F86" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="20" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D87" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F87" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="20" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D88" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E88" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F88" s="22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="20" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D89" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E89" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F89" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="20" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D90" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E90" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F90" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="20" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D91" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E91" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F91" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="20" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D92" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E92" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F92" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="20" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D93" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E93" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F93" s="22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="20" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D94" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E94" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F94" s="22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="20" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D95" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E95" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F95" s="22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="20" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D96" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E96" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F96" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="20" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D97" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E97" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F97" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="20" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="C98" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D98" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E98" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F98" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="20" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C99" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D99" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E99" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F99" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="20" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D100" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E100" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F100" s="22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="20" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D101" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E101" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F101" s="22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="20" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D102" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E102" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F102" s="22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="20" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D103" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E103" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F103" s="22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="20" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C104" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D104" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E104" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F104" s="22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="20" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C105" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D105" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E105" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F105" s="22" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3544,452 +4333,452 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B2:B105 C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+        <v>184</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="24" t="n">
+      <c r="A2" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="25" t="n">
         <v>3.382628</v>
       </c>
-      <c r="C2" s="24" t="n">
+      <c r="C2" s="25" t="n">
         <v>36.738027</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="24" t="n">
+      <c r="A3" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="25" t="n">
         <v>3.796547</v>
       </c>
-      <c r="C3" s="24" t="n">
+      <c r="C3" s="25" t="n">
         <v>36.452382</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="24" t="n">
+      <c r="A4" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="25" t="n">
         <v>3.656768</v>
       </c>
-      <c r="C4" s="24" t="n">
+      <c r="C4" s="25" t="n">
         <v>36.834157</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" s="24" t="n">
+      <c r="A5" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="25" t="n">
         <v>4.223964</v>
       </c>
-      <c r="C5" s="24" t="n">
+      <c r="C5" s="25" t="n">
         <v>36.759999</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" s="24" t="n">
+      <c r="A6" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="25" t="n">
         <v>3.560828</v>
       </c>
-      <c r="C6" s="24" t="n">
+      <c r="C6" s="25" t="n">
         <v>36.606191</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" s="24" t="n">
+      <c r="A7" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="25" t="n">
         <v>3.708845</v>
       </c>
-      <c r="C7" s="24" t="n">
+      <c r="C7" s="25" t="n">
         <v>36.438639</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="B8" s="24" t="n">
+      <c r="A8" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="25" t="n">
         <v>3.48036943</v>
       </c>
-      <c r="C8" s="24" t="n">
+      <c r="C8" s="25" t="n">
         <v>36.8153996</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="B9" s="24" t="n">
+      <c r="A9" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="25" t="n">
         <v>3.81834414</v>
       </c>
-      <c r="C9" s="24" t="n">
+      <c r="C9" s="25" t="n">
         <v>36.5419431</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" s="24" t="n">
+      <c r="A10" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="25" t="n">
         <v>3.68687441</v>
       </c>
-      <c r="C10" s="24" t="n">
+      <c r="C10" s="25" t="n">
         <v>36.8941092</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="B11" s="24" t="n">
+      <c r="A11" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" s="25" t="n">
         <v>4.22586571</v>
       </c>
-      <c r="C11" s="24" t="n">
+      <c r="C11" s="25" t="n">
         <v>36.7745918</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" s="24" t="n">
+      <c r="A12" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="25" t="n">
         <v>3.62335251</v>
       </c>
-      <c r="C12" s="24" t="n">
+      <c r="C12" s="25" t="n">
         <v>36.6454257</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" s="24" t="n">
+      <c r="A13" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="25" t="n">
         <v>3.74291712</v>
       </c>
-      <c r="C13" s="24" t="n">
+      <c r="C13" s="25" t="n">
         <v>36.5148909</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="B14" s="24" t="n">
+      <c r="A14" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" s="25" t="n">
         <v>3.57735223</v>
       </c>
-      <c r="C14" s="24" t="n">
+      <c r="C14" s="25" t="n">
         <v>36.8301506</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="B15" s="24" t="n">
+      <c r="A15" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" s="25" t="n">
         <v>3.83814888</v>
       </c>
-      <c r="C15" s="24" t="n">
+      <c r="C15" s="25" t="n">
         <v>36.5714184</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="B16" s="24" t="n">
+      <c r="A16" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="B16" s="25" t="n">
         <v>3.7143189</v>
       </c>
-      <c r="C16" s="24" t="n">
+      <c r="C16" s="25" t="n">
         <v>36.9938681</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="B17" s="24" t="n">
+      <c r="A17" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="25" t="n">
         <v>4.23442864</v>
       </c>
-      <c r="C17" s="24" t="n">
+      <c r="C17" s="25" t="n">
         <v>36.7821268</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="B18" s="24" t="n">
+      <c r="A18" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="25" t="n">
         <v>3.66715437</v>
       </c>
-      <c r="C18" s="24" t="n">
+      <c r="C18" s="25" t="n">
         <v>36.6733122</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="B19" s="24" t="n">
+      <c r="A19" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="25" t="n">
         <v>3.75223271</v>
       </c>
-      <c r="C19" s="24" t="n">
+      <c r="C19" s="25" t="n">
         <v>36.5612685</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="B20" s="24" t="n">
+      <c r="A20" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" s="25" t="n">
         <v>3.67597052</v>
       </c>
-      <c r="C20" s="24" t="n">
+      <c r="C20" s="25" t="n">
         <v>36.8464066</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="B21" s="24" t="n">
+      <c r="A21" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="25" t="n">
         <v>3.87715608</v>
       </c>
-      <c r="C21" s="24" t="n">
+      <c r="C21" s="25" t="n">
         <v>36.633536</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="B22" s="24" t="n">
+      <c r="A22" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" s="25" t="n">
         <v>3.73961887</v>
       </c>
-      <c r="C22" s="24" t="n">
+      <c r="C22" s="25" t="n">
         <v>37.0495704</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="B23" s="24" t="n">
+      <c r="A23" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="B23" s="25" t="n">
         <v>4.32969441</v>
       </c>
-      <c r="C23" s="24" t="n">
+      <c r="C23" s="25" t="n">
         <v>36.8293979</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="B24" s="24" t="n">
+      <c r="A24" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="25" t="n">
         <v>3.68396877</v>
       </c>
-      <c r="C24" s="24" t="n">
+      <c r="C24" s="25" t="n">
         <v>36.7397901</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="B25" s="24" t="n">
+      <c r="A25" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="25" t="n">
         <v>3.82533597</v>
       </c>
-      <c r="C25" s="24" t="n">
+      <c r="C25" s="25" t="n">
         <v>36.64824</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="B26" s="24" t="n">
+      <c r="A26" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" s="25" t="n">
         <v>3.76064683</v>
       </c>
-      <c r="C26" s="24" t="n">
+      <c r="C26" s="25" t="n">
         <v>36.8839447</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="B27" s="24" t="n">
+      <c r="A27" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="25" t="n">
         <v>3.91718799</v>
       </c>
-      <c r="C27" s="24" t="n">
+      <c r="C27" s="25" t="n">
         <v>36.6690465</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="B28" s="24" t="n">
+      <c r="A28" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="B28" s="25" t="n">
         <v>3.7657132</v>
       </c>
-      <c r="C28" s="24" t="n">
+      <c r="C28" s="25" t="n">
         <v>37.0824723</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="B29" s="24" t="n">
+      <c r="A29" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="25" t="n">
         <v>4.35981594</v>
       </c>
-      <c r="C29" s="24" t="n">
+      <c r="C29" s="25" t="n">
         <v>36.8588089</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="B30" s="24" t="n">
+      <c r="A30" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="B30" s="25" t="n">
         <v>3.73594413</v>
       </c>
-      <c r="C30" s="24" t="n">
+      <c r="C30" s="25" t="n">
         <v>36.8315668</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="B31" s="24" t="n">
+      <c r="A31" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" s="25" t="n">
         <v>3.8771501</v>
       </c>
-      <c r="C31" s="24" t="n">
+      <c r="C31" s="25" t="n">
         <v>36.6973403</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="B32" s="24" t="n">
+      <c r="A32" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B32" s="25" t="n">
         <v>3.8330832</v>
       </c>
-      <c r="C32" s="24" t="n">
+      <c r="C32" s="25" t="n">
         <v>36.9110609</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="B33" s="24" t="n">
+      <c r="A33" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" s="25" t="n">
         <v>3.95505275</v>
       </c>
-      <c r="C33" s="24" t="n">
+      <c r="C33" s="25" t="n">
         <v>36.7655372</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="B34" s="24" t="n">
+      <c r="A34" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="B34" s="25" t="n">
         <v>3.85210038</v>
       </c>
-      <c r="C34" s="24" t="n">
+      <c r="C34" s="25" t="n">
         <v>37.1701443</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="B35" s="24" t="n">
+      <c r="A35" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="B35" s="25" t="n">
         <v>4.36048175</v>
       </c>
-      <c r="C35" s="24" t="n">
+      <c r="C35" s="25" t="n">
         <v>36.8803902</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="B36" s="24" t="n">
+      <c r="A36" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B36" s="25" t="n">
         <v>3.80123012</v>
       </c>
-      <c r="C36" s="24" t="n">
+      <c r="C36" s="25" t="n">
         <v>36.8774042</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B37" s="24" t="n">
+      <c r="A37" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" s="25" t="n">
         <v>3.95801733</v>
       </c>
-      <c r="C37" s="24" t="n">
+      <c r="C37" s="25" t="n">
         <v>36.7709093</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="B38" s="24" t="n">
+      <c r="A38" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="B38" s="25" t="n">
         <v>3.88537781</v>
       </c>
-      <c r="C38" s="24" t="n">
+      <c r="C38" s="25" t="n">
         <v>36.9964433</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="B39" s="24" t="n">
+      <c r="A39" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39" s="25" t="n">
         <v>4.02159372</v>
       </c>
-      <c r="C39" s="24" t="n">
+      <c r="C39" s="25" t="n">
         <v>36.8570698</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="B40" s="24" t="n">
+      <c r="A40" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B40" s="25" t="n">
         <v>3.88341944</v>
       </c>
-      <c r="C40" s="24" t="n">
+      <c r="C40" s="25" t="n">
         <v>37.2204854</v>
       </c>
     </row>

</xml_diff>